<commit_message>
nouvel essai invariant b4d169be6d2b60e7dc2d44c1180a961d5674d6a5
</commit_message>
<xml_diff>
--- a/VoitureBalaisDecisions/ig/StructureDefinition-FrSimpleQuantityMedication.xlsx
+++ b/VoitureBalaisDecisions/ig/StructureDefinition-FrSimpleQuantityMedication.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-08-13T14:38:26+00:00</t>
+    <t>2025-08-13T16:08:05+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -267,7 +267,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-qty-3:If a code for the unit is present, the system SHALL also be present {code.empty() or system.exists()}sqty-1:The comparator is not used on a SimpleQuantity {comparator.empty()}fr-med-smpl-quant-1:system SHALL be UCUM or EDQM if code is used {code.exists() and (system = `http://standardterms.edqm.eu` or system = `http://unitsofmeasure.org`)}fr-med-smpl-quant-2:system SHALL not be used if code is not used {code.empty() and system.empty()}</t>
+qty-3:If a code for the unit is present, the system SHALL also be present {code.empty() or system.exists()}sqty-1:The comparator is not used on a SimpleQuantity {comparator.empty()}fr-med-smpl-quant-1:system SHALL be UCUM or EDQM if code is used {code.exists() implies (system = `http://standardterms.edqm.eu` or system = `http://unitsofmeasure.org`)}fr-med-smpl-quant-2:system SHALL not be used if code is not used {code.empty() implies system.empty()}</t>
   </si>
   <si>
     <t>SN (see also Range) or CQ</t>

</xml_diff>

<commit_message>
essai rafinement invariant a5e796c516367093095fd220c0e40797fcd57fe7
</commit_message>
<xml_diff>
--- a/VoitureBalaisDecisions/ig/StructureDefinition-FrSimpleQuantityMedication.xlsx
+++ b/VoitureBalaisDecisions/ig/StructureDefinition-FrSimpleQuantityMedication.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-08-13T16:08:05+00:00</t>
+    <t>2025-08-13T16:43:50+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -267,7 +267,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-qty-3:If a code for the unit is present, the system SHALL also be present {code.empty() or system.exists()}sqty-1:The comparator is not used on a SimpleQuantity {comparator.empty()}fr-med-smpl-quant-1:system SHALL be UCUM or EDQM if code is used {code.exists() implies (system = `http://standardterms.edqm.eu` or system = `http://unitsofmeasure.org`)}fr-med-smpl-quant-2:system SHALL not be used if code is not used {code.empty() implies system.empty()}</t>
+qty-3:If a code for the unit is present, the system SHALL also be present {code.empty() or system.exists()}sqty-1:The comparator is not used on a SimpleQuantity {comparator.empty()}fr-med-smpl-quant-1:system SHALL be UCUM or EDQM if code is used {code.exists() implies (system.exists() and (system = `http://standardterms.edqm.eu` or system = `http://unitsofmeasure.org`))}fr-med-smpl-quant-2:system SHALL not be used if code is not used {code.empty() implies system.empty()}</t>
   </si>
   <si>
     <t>SN (see also Range) or CQ</t>

</xml_diff>

<commit_message>
correction magic tild (qui n'est pas si magique que ça) a50ed53d76f70cc0c8e56a3bc1bc7c1879d08a81
</commit_message>
<xml_diff>
--- a/VoitureBalaisDecisions/ig/StructureDefinition-FrSimpleQuantityMedication.xlsx
+++ b/VoitureBalaisDecisions/ig/StructureDefinition-FrSimpleQuantityMedication.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-08-19T07:49:07+00:00</t>
+    <t>2025-08-19T08:39:15+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -267,7 +267,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-qty-3:If a code for the unit is present, the system SHALL also be present {code.empty() or system.exists()}sqty-1:The comparator is not used on a SimpleQuantity {comparator.empty()}fr-med-smpl-quant-1:system SHALL be UCUM or EDQM if code is used {code.exists() implies (system.exists() and (system = `http://standardterms.edqm.eu` or system = `http://unitsofmeasure.org`))}fr-med-smpl-quant-2:system SHALL not be used if code is not used {code.empty() implies system.empty()}</t>
+qty-3:If a code for the unit is present, the system SHALL also be present {code.empty() or system.exists()}sqty-1:The comparator is not used on a SimpleQuantity {comparator.empty()}fr-med-smpl-quant-1:system SHALL be UCUM or EDQM if code is used {code.exists() implies (system.exists() and (system = 'http://standardterms.edqm.eu' or system = 'http://unitsofmeasure.org'))}fr-med-smpl-quant-2:system SHALL not be used if code is not used {code.empty() implies system.empty()}</t>
   </si>
   <si>
     <t>SN (see also Range) or CQ</t>

</xml_diff>